<commit_message>
new excel file added some imports errors resolved
</commit_message>
<xml_diff>
--- a/new-excel-file.xlsx
+++ b/new-excel-file.xlsx
@@ -23,613 +23,613 @@
     <t>File</t>
   </si>
   <si>
-    <t>SFRAZ-1</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-1</t>
-  </si>
-  <si>
-    <t>SFRAZ-2</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-2</t>
-  </si>
-  <si>
-    <t>SFRAZ-3</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-3</t>
-  </si>
-  <si>
-    <t>SFRAZ-4</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-4</t>
-  </si>
-  <si>
-    <t>SFRAZ-5</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-5</t>
-  </si>
-  <si>
-    <t>SFRAZ-6</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-6</t>
-  </si>
-  <si>
-    <t>SFRAZ-7</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-7</t>
-  </si>
-  <si>
-    <t>SFRAZ-8</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-8</t>
-  </si>
-  <si>
-    <t>SFRAZ-9</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-9</t>
-  </si>
-  <si>
-    <t>SFRAZ-10</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-10</t>
-  </si>
-  <si>
-    <t>SFRAZ-11</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-11</t>
-  </si>
-  <si>
-    <t>SFRAZ-12</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-12</t>
+    <t>TAG-1</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-1</t>
+  </si>
+  <si>
+    <t>TAG-2</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-2</t>
+  </si>
+  <si>
+    <t>TAG-3</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-3</t>
+  </si>
+  <si>
+    <t>TAG-4</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-4</t>
+  </si>
+  <si>
+    <t>TAG-5</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-5</t>
+  </si>
+  <si>
+    <t>TAG-6</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-6</t>
+  </si>
+  <si>
+    <t>TAG-7</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-7</t>
+  </si>
+  <si>
+    <t>TAG-8</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-8</t>
+  </si>
+  <si>
+    <t>TAG-9</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-9</t>
+  </si>
+  <si>
+    <t>TAG-10</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-10</t>
+  </si>
+  <si>
+    <t>TAG-11</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-11</t>
+  </si>
+  <si>
+    <t>TAG-12</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-12</t>
   </si>
   <si>
     <t>Category from 12</t>
   </si>
   <si>
-    <t>SFRAZ-13</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-13</t>
-  </si>
-  <si>
-    <t>SFRAZ-14</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-14</t>
-  </si>
-  <si>
-    <t>SFRAZ-15</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-15</t>
-  </si>
-  <si>
-    <t>SFRAZ-16</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-16</t>
-  </si>
-  <si>
-    <t>SFRAZ-17</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-17</t>
-  </si>
-  <si>
-    <t>SFRAZ-18</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-18</t>
-  </si>
-  <si>
-    <t>SFRAZ-19</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-19</t>
-  </si>
-  <si>
-    <t>SFRAZ-20</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-20</t>
-  </si>
-  <si>
-    <t>SFRAZ-21</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-21</t>
-  </si>
-  <si>
-    <t>SFRAZ-22</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-22</t>
-  </si>
-  <si>
-    <t>SFRAZ-23</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-23</t>
-  </si>
-  <si>
-    <t>SFRAZ-24</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-24</t>
-  </si>
-  <si>
-    <t>SFRAZ-25</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-25</t>
-  </si>
-  <si>
-    <t>SFRAZ-26</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-26</t>
-  </si>
-  <si>
-    <t>SFRAZ-27</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-27</t>
-  </si>
-  <si>
-    <t>SFRAZ-28</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-28</t>
-  </si>
-  <si>
-    <t>SFRAZ-29</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-29</t>
-  </si>
-  <si>
-    <t>SFRAZ-30</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-30</t>
+    <t>TAG-13</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-13</t>
+  </si>
+  <si>
+    <t>TAG-14</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-14</t>
+  </si>
+  <si>
+    <t>TAG-15</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-15</t>
+  </si>
+  <si>
+    <t>TAG-16</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-16</t>
+  </si>
+  <si>
+    <t>TAG-17</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-17</t>
+  </si>
+  <si>
+    <t>TAG-18</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-18</t>
+  </si>
+  <si>
+    <t>TAG-19</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-19</t>
+  </si>
+  <si>
+    <t>TAG-20</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-20</t>
+  </si>
+  <si>
+    <t>TAG-21</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-21</t>
+  </si>
+  <si>
+    <t>TAG-22</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-22</t>
+  </si>
+  <si>
+    <t>TAG-23</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-23</t>
+  </si>
+  <si>
+    <t>TAG-24</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-24</t>
+  </si>
+  <si>
+    <t>TAG-25</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-25</t>
+  </si>
+  <si>
+    <t>TAG-26</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-26</t>
+  </si>
+  <si>
+    <t>TAG-27</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-27</t>
+  </si>
+  <si>
+    <t>TAG-28</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-28</t>
+  </si>
+  <si>
+    <t>TAG-29</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-29</t>
+  </si>
+  <si>
+    <t>TAG-30</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-30</t>
   </si>
   <si>
     <t>Category from 30</t>
   </si>
   <si>
-    <t>SFRAZ-31</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-31</t>
-  </si>
-  <si>
-    <t>SFRAZ-32</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-32</t>
-  </si>
-  <si>
-    <t>SFRAZ-33</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-33</t>
-  </si>
-  <si>
-    <t>SFRAZ-34</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-34</t>
-  </si>
-  <si>
-    <t>SFRAZ-35</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-35</t>
-  </si>
-  <si>
-    <t>SFRAZ-36</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-36</t>
-  </si>
-  <si>
-    <t>SFRAZ-37</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-37</t>
-  </si>
-  <si>
-    <t>SFRAZ-38</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-38</t>
-  </si>
-  <si>
-    <t>SFRAZ-39</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-39</t>
-  </si>
-  <si>
-    <t>SFRAZ-40</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-40</t>
-  </si>
-  <si>
-    <t>SFRAZ-41</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-41</t>
-  </si>
-  <si>
-    <t>SFRAZ-42</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-42</t>
-  </si>
-  <si>
-    <t>SFRAZ-43</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-43</t>
-  </si>
-  <si>
-    <t>SFRAZ-44</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-44</t>
-  </si>
-  <si>
-    <t>SFRAZ-45</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-45</t>
-  </si>
-  <si>
-    <t>SFRAZ-46</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-46</t>
-  </si>
-  <si>
-    <t>SFRAZ-47</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-47</t>
-  </si>
-  <si>
-    <t>SFRAZ-48</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-48</t>
-  </si>
-  <si>
-    <t>SFRAZ-49</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-49</t>
-  </si>
-  <si>
-    <t>SFRAZ-50</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-50</t>
-  </si>
-  <si>
-    <t>SFRAZ-51</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-51</t>
-  </si>
-  <si>
-    <t>SFRAZ-52</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-52</t>
-  </si>
-  <si>
-    <t>SFRAZ-53</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-53</t>
-  </si>
-  <si>
-    <t>SFRAZ-54</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-54</t>
-  </si>
-  <si>
-    <t>SFRAZ-55</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-55</t>
-  </si>
-  <si>
-    <t>SFRAZ-56</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-56</t>
-  </si>
-  <si>
-    <t>SFRAZ-57</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-57</t>
-  </si>
-  <si>
-    <t>SFRAZ-58</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-58</t>
-  </si>
-  <si>
-    <t>SFRAZ-59</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-59</t>
-  </si>
-  <si>
-    <t>SFRAZ-60</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-60</t>
-  </si>
-  <si>
-    <t>SFRAZ-61</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-61</t>
-  </si>
-  <si>
-    <t>SFRAZ-62</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-62</t>
-  </si>
-  <si>
-    <t>SFRAZ-63</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-63</t>
-  </si>
-  <si>
-    <t>SFRAZ-64</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-64</t>
-  </si>
-  <si>
-    <t>SFRAZ-65</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-65</t>
-  </si>
-  <si>
-    <t>SFRAZ-66</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-66</t>
-  </si>
-  <si>
-    <t>SFRAZ-67</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-67</t>
-  </si>
-  <si>
-    <t>SFRAZ-68</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-68</t>
-  </si>
-  <si>
-    <t>SFRAZ-69</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-69</t>
-  </si>
-  <si>
-    <t>SFRAZ-70</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-70</t>
+    <t>TAG-31</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-31</t>
+  </si>
+  <si>
+    <t>TAG-32</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-32</t>
+  </si>
+  <si>
+    <t>TAG-33</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-33</t>
+  </si>
+  <si>
+    <t>TAG-34</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-34</t>
+  </si>
+  <si>
+    <t>TAG-35</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-35</t>
+  </si>
+  <si>
+    <t>TAG-36</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-36</t>
+  </si>
+  <si>
+    <t>TAG-37</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-37</t>
+  </si>
+  <si>
+    <t>TAG-38</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-38</t>
+  </si>
+  <si>
+    <t>TAG-39</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-39</t>
+  </si>
+  <si>
+    <t>TAG-40</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-40</t>
+  </si>
+  <si>
+    <t>TAG-41</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-41</t>
+  </si>
+  <si>
+    <t>TAG-42</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-42</t>
+  </si>
+  <si>
+    <t>TAG-43</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-43</t>
+  </si>
+  <si>
+    <t>TAG-44</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-44</t>
+  </si>
+  <si>
+    <t>TAG-45</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-45</t>
+  </si>
+  <si>
+    <t>TAG-46</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-46</t>
+  </si>
+  <si>
+    <t>TAG-47</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-47</t>
+  </si>
+  <si>
+    <t>TAG-48</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-48</t>
+  </si>
+  <si>
+    <t>TAG-49</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-49</t>
+  </si>
+  <si>
+    <t>TAG-50</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-50</t>
+  </si>
+  <si>
+    <t>TAG-51</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-51</t>
+  </si>
+  <si>
+    <t>TAG-52</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-52</t>
+  </si>
+  <si>
+    <t>TAG-53</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-53</t>
+  </si>
+  <si>
+    <t>TAG-54</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-54</t>
+  </si>
+  <si>
+    <t>TAG-55</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-55</t>
+  </si>
+  <si>
+    <t>TAG-56</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-56</t>
+  </si>
+  <si>
+    <t>TAG-57</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-57</t>
+  </si>
+  <si>
+    <t>TAG-58</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-58</t>
+  </si>
+  <si>
+    <t>TAG-59</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-59</t>
+  </si>
+  <si>
+    <t>TAG-60</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-60</t>
+  </si>
+  <si>
+    <t>TAG-61</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-61</t>
+  </si>
+  <si>
+    <t>TAG-62</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-62</t>
+  </si>
+  <si>
+    <t>TAG-63</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-63</t>
+  </si>
+  <si>
+    <t>TAG-64</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-64</t>
+  </si>
+  <si>
+    <t>TAG-65</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-65</t>
+  </si>
+  <si>
+    <t>TAG-66</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-66</t>
+  </si>
+  <si>
+    <t>TAG-67</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-67</t>
+  </si>
+  <si>
+    <t>TAG-68</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-68</t>
+  </si>
+  <si>
+    <t>TAG-69</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-69</t>
+  </si>
+  <si>
+    <t>TAG-70</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-70</t>
   </si>
   <si>
     <t>Category from 70</t>
   </si>
   <si>
-    <t>SFRAZ-71</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-71</t>
-  </si>
-  <si>
-    <t>SFRAZ-72</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-72</t>
-  </si>
-  <si>
-    <t>SFRAZ-73</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-73</t>
-  </si>
-  <si>
-    <t>SFRAZ-74</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-74</t>
-  </si>
-  <si>
-    <t>SFRAZ-75</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-75</t>
-  </si>
-  <si>
-    <t>SFRAZ-76</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-76</t>
-  </si>
-  <si>
-    <t>SFRAZ-77</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-77</t>
-  </si>
-  <si>
-    <t>SFRAZ-78</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-78</t>
-  </si>
-  <si>
-    <t>SFRAZ-79</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-79</t>
-  </si>
-  <si>
-    <t>SFRAZ-80</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-80</t>
-  </si>
-  <si>
-    <t>SFRAZ-81</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-81</t>
-  </si>
-  <si>
-    <t>SFRAZ-82</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-82</t>
-  </si>
-  <si>
-    <t>SFRAZ-83</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-83</t>
-  </si>
-  <si>
-    <t>SFRAZ-84</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-84</t>
-  </si>
-  <si>
-    <t>SFRAZ-85</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-85</t>
-  </si>
-  <si>
-    <t>SFRAZ-86</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-86</t>
-  </si>
-  <si>
-    <t>SFRAZ-87</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-87</t>
-  </si>
-  <si>
-    <t>SFRAZ-88</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-88</t>
-  </si>
-  <si>
-    <t>SFRAZ-89</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-89</t>
-  </si>
-  <si>
-    <t>SFRAZ-90</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-90</t>
-  </si>
-  <si>
-    <t>SFRAZ-91</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-91</t>
-  </si>
-  <si>
-    <t>SFRAZ-92</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-92</t>
-  </si>
-  <si>
-    <t>SFRAZ-93</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-93</t>
-  </si>
-  <si>
-    <t>SFRAZ-94</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-94</t>
-  </si>
-  <si>
-    <t>SFRAZ-95</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-95</t>
-  </si>
-  <si>
-    <t>SFRAZ-96</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-96</t>
-  </si>
-  <si>
-    <t>SFRAZ-97</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-97</t>
-  </si>
-  <si>
-    <t>SFRAZ-98</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-98</t>
-  </si>
-  <si>
-    <t>SFRAZ-99</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-99</t>
-  </si>
-  <si>
-    <t>SFRAZ-100</t>
-  </si>
-  <si>
-    <t>Scenario: This is a long scenario description for the tag: SFRAZ-100</t>
+    <t>TAG-71</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-71</t>
+  </si>
+  <si>
+    <t>TAG-72</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-72</t>
+  </si>
+  <si>
+    <t>TAG-73</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-73</t>
+  </si>
+  <si>
+    <t>TAG-74</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-74</t>
+  </si>
+  <si>
+    <t>TAG-75</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-75</t>
+  </si>
+  <si>
+    <t>TAG-76</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-76</t>
+  </si>
+  <si>
+    <t>TAG-77</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-77</t>
+  </si>
+  <si>
+    <t>TAG-78</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-78</t>
+  </si>
+  <si>
+    <t>TAG-79</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-79</t>
+  </si>
+  <si>
+    <t>TAG-80</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-80</t>
+  </si>
+  <si>
+    <t>TAG-81</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-81</t>
+  </si>
+  <si>
+    <t>TAG-82</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-82</t>
+  </si>
+  <si>
+    <t>TAG-83</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-83</t>
+  </si>
+  <si>
+    <t>TAG-84</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-84</t>
+  </si>
+  <si>
+    <t>TAG-85</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-85</t>
+  </si>
+  <si>
+    <t>TAG-86</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-86</t>
+  </si>
+  <si>
+    <t>TAG-87</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-87</t>
+  </si>
+  <si>
+    <t>TAG-88</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-88</t>
+  </si>
+  <si>
+    <t>TAG-89</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-89</t>
+  </si>
+  <si>
+    <t>TAG-90</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-90</t>
+  </si>
+  <si>
+    <t>TAG-91</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-91</t>
+  </si>
+  <si>
+    <t>TAG-92</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-92</t>
+  </si>
+  <si>
+    <t>TAG-93</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-93</t>
+  </si>
+  <si>
+    <t>TAG-94</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-94</t>
+  </si>
+  <si>
+    <t>TAG-95</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-95</t>
+  </si>
+  <si>
+    <t>TAG-96</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-96</t>
+  </si>
+  <si>
+    <t>TAG-97</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-97</t>
+  </si>
+  <si>
+    <t>TAG-98</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-98</t>
+  </si>
+  <si>
+    <t>TAG-99</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-99</t>
+  </si>
+  <si>
+    <t>TAG-100</t>
+  </si>
+  <si>
+    <t>Scenario: This is a long scenario description for the tag: TAG-100</t>
   </si>
 </sst>
 </file>
@@ -690,8 +690,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="11.20703125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="63.01953125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="8.99609375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="60.8125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="17.22265625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>

</xml_diff>